<commit_message>
Finalmente consegui ajeitar essa função de geração da planilha, foi um processo brutal
</commit_message>
<xml_diff>
--- a/results/resultados_tratamento.xlsx
+++ b/results/resultados_tratamento.xlsx
@@ -7,31 +7,29 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4. COMO VOCÊ CLASSIFICARIA O S" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6. SE AS ELEIÇÕES PARA PREFEIT" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="7. INDEPENDENTE DA SUA INTENÇÃ" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="8. INDEPENDENTE DA SUA INTENÇÃ" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="9. EM RELAÇÃO A SUA INTENÇÃO D" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="10. SOBRE A CANDIDATURA A PREF" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11. (EXCETO PARA QUEM NÃO CONH" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="12. SOBRE A CANDIDATURA A PREF" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="13. (EXCETO PARA QUEM NÃO O CO" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="14. SOBRE A CANDIDATURA A PREF" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="15. (EXCETO PARA QUEM NÃO O CO" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="16. SE AS ELEIÇÕES PARA PREFEI" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="18. SE AS ELEIÇÕES PARA PREFEI" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="19. DE MANEIRA GERAL, COMO VOC" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20. SOBRE A GESTÃO DA PREFEITA" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="21. DE MANEIRA GERAL, SOBRE A " sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="22. EM QUAL DESSES CANDIDATOS " sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="23. (NÃO PEA) DAS ALTERNATIVAS" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="24. RENDA (PESSOAL)" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="25. RELIGIÃO" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1. SEXO" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2. FAIXA ETÁRIA" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3. ESCOLARIDADE" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="5. SE AS ELEIÇÕES PARA PREFEIT" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="17. A PREFEITA NADEGI NÃO PODE" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Espontanea_25. RELIGI" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Espontanea_5. SE AS E" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Espontanea_17. A PREF" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_4. COMO VO" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_6. SE AS E" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_7. INDEPEN" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_8. INDEPEN" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_9. EM RELA" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_10. SOBRE " sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_11. (EXCET" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_12. SOBRE " sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_13. (EXCET" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_14. SOBRE " sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_15. (EXCET" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_16. SE AS " sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_18. SE AS " sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_19. DE MAN" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_20. SOBRE " sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_21. DE MAN" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_22. EM QUA" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_23. (NÃO P" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_24. RENDA " sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Estimulada_25. RELIGI" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -449,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,70 +458,105 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>25. RELIGIÃO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>17</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30.36%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>CATÓLICA</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>48.21%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>15</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>26.79%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>EVANGÉLICA</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>19</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>33.93%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>11</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>19.64%</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>ESPÍRITA</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>7</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12.5%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>10</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>17.86%</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>SEM RELIGIÃO</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3.57%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>3</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>5.36%</t>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1.79%</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>56</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -540,7 +573,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -551,70 +584,90 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>11. (EXCETO PARA QUEM NÃO CONHECE) E VOCÊ POSSUI UMA IMAGEM POSITIVA OU NEGATIVA DO PRÉ-CANDIDATO A PREFEITO DE CAMARAGIBE DIEGO CABRAL: (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>27</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>48.21%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>POSITIVA</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>42.86%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>NEM POSITIVA NEM NEGATIVA</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>18</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>32.14%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>9</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>16.07%</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>12</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>21.43%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1.79%</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>NEGATIVA</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3.57%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1.79%</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>56</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -631,7 +684,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -642,60 +695,105 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>12. SOBRE A CANDIDATURA A PREFEITO DE CAMARAGIBE DE JORGE ALEXANDRE, VOCÊ DIRIA QUE: (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>22</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>39.29%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>16</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>28.57%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>20</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>35.71%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>NÃO VOTARIA DE JEITO NENHUM</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>14</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>25.0%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>13</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>23.21%</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>VOTARIA COM CERTEZA</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>12</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>21.43%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1.79%</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>TALVEZ VOTARIA</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>8</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>14.29%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>NÃO O CONHECE O SUFICIENTE PARA OPINAR</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10.71%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>56</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -712,7 +810,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -723,80 +821,90 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>13. (EXCETO PARA QUEM NÃO O CONHECE) E VOCÊ POSSUI UMA IMAGEM POSITIVA OU NEGATIVA DO PRÉ-CANDIDATO A PREFEITO DE CAMARAGIBE JORGE ALEXANDRE: (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>23</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>41.07%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>NEM POSITIVA NEM NEGATIVA</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>20</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>35.71%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>POSITIVA</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>14</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>25.0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>13</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>23.21%</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>10</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>17.86%</t>
-        </is>
-      </c>
-    </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>5</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>8.93%</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>NEGATIVA</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>9</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>16.07%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>7.14%</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1.79%</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>56</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -813,7 +921,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -824,70 +932,105 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>14. SOBRE A CANDIDATURA A PREFEITO DE CAMARAGIBE DE BOSCO, VOCÊ DIRIA QUE: (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>23</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>41.07%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>NÃO VOTARIA DE JEITO NENHUM</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>48.21%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>18</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>32.14%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>11</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>19.64%</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>NÃO O CONHECE O SUFICIENTE PARA OPINAR</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>16.07%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>5.36%</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>VOTARIA COM CERTEZA</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1.79%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>TALVEZ VOTARIA</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>1</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>1.79%</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>56</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -904,7 +1047,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -915,50 +1058,90 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>15. (EXCETO PARA QUEM NÃO O CONHECE) E VOCÊ POSSUI UMA IMAGEM POSITIVA OU NEGATIVA DO PRÉ-CANDIDATO A PREFEITO DE CAMARAGIBE BOSCO: (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>23</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>41.07%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>NEM POSITIVA NEM NEGATIVA</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>22</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>39.29%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>22</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>39.29%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>35.71%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>11</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>19.64%</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>NEGATIVA</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>13</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>23.21%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>POSITIVA</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1.79%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>56</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -975,7 +1158,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -986,80 +1169,120 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>16. SE AS ELEIÇÕES PARA PREFEITO DE CAMARAGIBE FOSSEM HOJE, EM QUEM VOCÊ VOTARIA? (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>16</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>28.57%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>DIEGO CABRAL, APOIADO PELO PREFEITO DE RECIFE JOÃO CAMPOS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>23</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>41.07%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>12</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>21.43%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>JORGE ALEXANDRE, APOIADO POR MARCELO GOUVEIA</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>13</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>23.21%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>11</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>19.64%</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>17.86%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>8</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>14.29%</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>FELIPE DANTAS, APOIADO POR ANDERSON FERREIRA</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>8.93%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>6</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>10.71%</t>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>NENHUM DELES</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>7.14%</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>5.36%</t>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>BOSCO, APOIADO POR DUDU DA FONTE</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1.79%</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>56</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -1076,7 +1299,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1087,50 +1310,105 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>18. SE AS ELEIÇÕES PARA PREFEITO DE CAMARAGIBE FOSSEM HOJE, VOCÊ VOTARIA EM DIEGO CABRAL SE O PRESIDENTE LULA APOIAR? (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>30</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>53.57%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SOU INFLUENCIADO PELO APOIO DE LULA</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>23</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>41.07%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>VOTARIA COM CERTEZA</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>18</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>32.14%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>8</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>14.29%</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>11</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>19.64%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>NÃO VOTARIA DE JEITO NENHUM</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>5.36%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>TALVEZ VOTARIA</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1.79%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>56</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -1147,7 +1425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1158,80 +1436,75 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>19. DE MANEIRA GERAL, COMO VOCÊ AVALIA A GESTÃO DA GOVERNADORA RAQUEL LYRA? (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>17</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>30.36%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>DESAPROVO</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>23</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>41.07%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>14</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>25.0%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>APROVO</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>22</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>39.29%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>10</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>17.86%</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>11</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>19.64%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>7</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>12.5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>8.93%</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>5.36%</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>56</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -1248,7 +1521,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1259,70 +1532,120 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>20. SOBRE A GESTÃO DA PREFEITA NADEGI, COMO O (A) SR. (A) AVALIA A SUA ADMINISTRAÇÃO A FRENTE DA PREFEITURA DE CAMARAGIBE? (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>22</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>39.29%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>RUIM</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>16</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>28.57%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>17</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>30.36%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>PÉSSIMA</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>21.43%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>9</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>16.07%</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>BOA</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>11</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>19.64%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>7</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>12.5%</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>8</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>14.29%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1.79%</t>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>REGULAR</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10.71%</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>ÓTIMA</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>5.36%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>56</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -1339,7 +1662,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1350,60 +1673,75 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>21. DE MANEIRA GERAL, SOBRE A FORMA DE ADMINISTRAR DA PREFEITA NADEGI, O (A) SR. (A) APROVA OU DESAPROVA? (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>37</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>66.07%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>DESAPROVO</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>30</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>53.57%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>10</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>17.86%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>APROVO</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>18</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>32.14%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>8</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>14.29%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1.79%</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>56</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -1420,7 +1758,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1431,80 +1769,105 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>5. SE AS ELEIÇÕES PARA PREFEITO DE CAMARAGIBE FOSSE HOJE, EM QUAL CANDIDATO VOCÊ VOTARIA? (RU ESPONTÂNEA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>24</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>42.86%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>DIEGO CABRAL</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>22</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>39.29%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>JORGE ALEXANDRE</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>14</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>25.0%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>NENHUM</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>7</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>12.5%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>FELIPE DANTAS</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>7</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>12.5%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>6</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>10.71%</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>7.14%</t>
-        </is>
-      </c>
-    </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1.79%</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>56</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -1521,7 +1884,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1532,70 +1895,120 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>22. EM QUAL DESSES CANDIDATOS VOCÊ NÃO VOTARIA DE MANEIRA ALGUMA? (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>27</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>48.21%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>BOSCO</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>17</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>30.36%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>19</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>33.93%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>14</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>25.0%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>JORGE ALEXANDRE</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>17.86%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>FELIPE DANTAS</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>7</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>12.5%</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>3.57%</t>
-        </is>
-      </c>
-    </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1.79%</t>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>NENHUM DELES</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>8.93%</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>DIEGO CABRAL</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>5.36%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>56</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -1612,7 +2025,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1623,40 +2036,105 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Contagem</t>
+          <t>23. (NÃO PEA) DAS ALTERNATIVAS QUE VOU LER, QUAL MELHOR REPRESENTA A SUA SITUAÇÃO EM RELAÇÃO AO TRABALHO?</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Porcentagem</t>
+          <t>contagem</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>33</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>58.93%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>APOSENTADO(A) OU NO SEGURO</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>22</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>39.29%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>23</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>41.07%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>DONA DE CASA QUE NÃO TRABALHA</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>17</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>30.36%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>DESEMPREGADO(A)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>16.07%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>ESTUDANTE QUE NÃO TRABALHA</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>7</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>12.5%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1.79%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>56</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -1673,7 +2151,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1684,80 +2162,90 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>24. RENDA (PESSOAL)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>15</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>26.79%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>ATÉ 1 SALÁRIO MÍNIMO</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>37</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>66.07%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>13</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>23.21%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>17.86%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>9</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>16.07%</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>DE 1 A 3 SALÁRIOS MÍNIMOS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>14.29%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>7</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>12.5%</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>DE 3 A 5 SALÁRIOS MÍNIMOS</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1.79%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>7</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>12.5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>8.93%</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>56</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -1774,7 +2262,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1785,252 +2273,105 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>25. RELIGIÃO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>31</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>55.36%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>CATÓLICA</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>27</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>48.21%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>15</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>26.79%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>EVANGÉLICA</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>19</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>33.93%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>8</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>14.29%</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>ESPÍRITA</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>7</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12.5%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>SEM RELIGIÃO</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>2</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>3.57%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1.79%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>56</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>100.00%</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>contagem</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>porcentagem</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>22</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>39.29%</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>14</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>25.0%</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>7</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>12.5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>7</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>12.5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>6</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>10.71%</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>56</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>100.00%</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>contagem</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>porcentagem</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>21</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>37.5%</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>20</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>35.71%</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>10</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>17.86%</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>5.36%</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1.79%</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1.79%</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>56</v>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -2047,7 +2388,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2058,80 +2399,120 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>17. A PREFEITA NADEGI NÃO PODERÁ SER MAIS CANDIDATA NA PRÓXIMA ELEIÇÃO. QUEM É O CANDIDATO A PREFEITO QUE ELA IRÁ APOIAR? (RU ESPONTÂNEA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>24</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>42.86%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>NENHUM</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>21</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>37.5%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>13</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>23.21%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>DIEGO CABRAL</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>35.71%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>7</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>12.5%</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>17.86%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>7</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>12.5%</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>FELIPE DANTAS</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>5.36%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>7.14%</t>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>BOSCO</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1.79%</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>JORGE ALEXANDRE</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>1</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>1.79%</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>56</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -2148,7 +2529,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2159,80 +2540,105 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>4. COMO VOCÊ CLASSIFICARIA O SEU INTERESSE NAS ELEIÇÕES MUNICIPAIS DESTE ANO? (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>24</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>42.86%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>INTERESSADO</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>17</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>30.36%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>13</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>23.21%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>POUCO INTERESSADO</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>26.79%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>7</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>12.5%</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>DESINTERESSADO</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>11</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>19.64%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>6</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>10.71%</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>MUITO INTERESSADO</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>10</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>17.86%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>8.93%</t>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>5.36%</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1.79%</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>56</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -2249,7 +2655,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2260,60 +2666,120 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>6. SE AS ELEIÇÕES PARA PREFEITO DE CAMARAGIBE FOSSEM HOJE, EM QUAIS DESSES CANDIDATOS VOCÊ VOTARIA? (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>47</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>83.93%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>DIEGO CABRAL</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>42.86%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>JORGE ALEXANDRE</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>14</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>25.0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>7</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12.5%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>FELIPE DANTAS</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>10.71%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>NENHUM DELES</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>4</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>7.14%</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>7.14%</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>BOSCO</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>1</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>1.79%</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>56</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -2330,7 +2796,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2341,70 +2807,120 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>7. INDEPENDENTE DA SUA INTENÇÃO DE VOTOS, QUEM VOCÊ ACREDITA QUE ESTEJA MAIS PREPARADO PARA SER PREFEITO DE CAMARAGIBE? (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>22</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>39.29%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>DIEGO CABRAL</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>42.86%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>15</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>26.79%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>JORGE ALEXANDRE</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>13</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>23.21%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>7</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>12.5%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>6</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>10.71%</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>FELIPE DANTAS</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>7</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>12.5%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>6</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>10.71%</t>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>NENHUM DELES</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>7.14%</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>BOSCO</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1.79%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>56</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -2421,7 +2937,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2432,60 +2948,120 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>8. INDEPENDENTE DA SUA INTENÇÃO DE VOTOS, QUEM VOCÊ ACREDITA QUE GANHARÁ A ELEIÇÃO PARA PREFEITO DE CAMARAGIBE? (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>DIEGO CABRAL</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>24</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>42.86%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>18</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>32.14%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>JORGE ALEXANDRE</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>13</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>23.21%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>12</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>21.43%</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>FELIPE DANTAS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>7</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12.5%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>3.57%</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>10.71%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>NENHUM DELES</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>8.93%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>BOSCO</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1.79%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>56</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -2502,7 +3078,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2513,70 +3089,90 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>9. EM RELAÇÃO A SUA INTENÇÃO DE VOTO PARA PREFEITO DE CAMARAGIBE, HOJE VOCÊ DIRIA QUE: (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>16</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>28.57%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>É DEFINITIVA, NÃO MUDAREI DE OPINIÃO</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>47</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>83.93%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>14</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>25.0%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>7.14%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>12</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>21.43%</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>NÃO É DEFINITIVA, MUDAREI DE OPINIÃO</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>7.14%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>8</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>14.29%</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>TALVEZ MUDAREI DE OPINIÃO</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1.79%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>6</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>10.71%</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>56</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>
@@ -2593,7 +3189,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2604,60 +3200,105 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>10. SOBRE A CANDIDATURA A PREFEITO DE CAMARAGIBE DE DIEGO CABRAL, VOCÊ DIRIA QUE: (RU ESTIMULADA)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>contagem</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>porcentagem</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>20</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>35.71%</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>VOTARIA COM CERTEZA</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>22</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>39.29%</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>14</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>25.0%</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>NÃO SABE/NÃO RESPONDEU</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>26.79%</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>13</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>23.21%</t>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>TALVEZ VOTARIA</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>7</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12.5%</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>9</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>16.07%</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>NÃO O CONHECE O SUFICIENTE PARA OPINAR</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>10.71%</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>NÃO VOTARIA DE JEITO NENHUM</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10.71%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>56</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>

</xml_diff>